<commit_message>
updated excel pictures and files and updated readme
</commit_message>
<xml_diff>
--- a/additional_files/EDV.xlsx
+++ b/additional_files/EDV.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\work\edv-lecture\additional_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lstoldt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B7F8F6-113F-47CC-A589-07F9570D3B64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{601B9D48-FB81-4778-83E0-754DD7F2B4AE}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,10 +46,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -87,13 +86,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -101,13 +100,13 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -126,7 +125,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -140,6 +139,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -273,46 +273,46 @@
                   <c:v>30.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87.652956595884419</c:v>
+                  <c:v>68.771115878765016</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>247.91999999999993</c:v>
+                  <c:v>152.61266147823576</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>701.22365276707524</c:v>
+                  <c:v>338.66870045454954</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1983.3599999999992</c:v>
+                  <c:v>751.5529023385152</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5609.789222136601</c:v>
+                  <c:v>1667.8003141576057</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15866.879999999992</c:v>
+                  <c:v>3701.0806281888808</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44878.313777092801</c:v>
+                  <c:v>8213.2121574001285</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>126935.03999999991</c:v>
+                  <c:v>18226.258954935332</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>359026.51021674235</c:v>
+                  <c:v>40446.601052798855</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1015480.3199999991</c:v>
+                  <c:v>89756.627554185528</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2872212.0817339383</c:v>
+                  <c:v>199182.42769977564</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8123842.5599999912</c:v>
+                  <c:v>442013.48229606345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ED70-4E6C-88BB-BD34554C1028}"/>
             </c:ext>
@@ -414,46 +414,46 @@
                   <c:v>36.880000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>104.31</c:v>
+                  <c:v>81.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>295.02</c:v>
+                  <c:v>181.61</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>834.46</c:v>
+                  <c:v>403.02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2360.1999999999998</c:v>
+                  <c:v>894.35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6675.65</c:v>
+                  <c:v>1984.68</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18881.59</c:v>
+                  <c:v>4404.29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53405.19</c:v>
+                  <c:v>9773.7199999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>151052.70000000001</c:v>
+                  <c:v>21689.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>427241.55</c:v>
+                  <c:v>48131.46</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1208421.58</c:v>
+                  <c:v>106810.39</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3417932.38</c:v>
+                  <c:v>237027.09</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9667372.6500000004</c:v>
+                  <c:v>525996.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-ED70-4E6C-88BB-BD34554C1028}"/>
             </c:ext>
@@ -469,11 +469,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="579685784"/>
-        <c:axId val="579679552"/>
+        <c:axId val="460767376"/>
+        <c:axId val="460766592"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="579685784"/>
+        <c:axId val="460767376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -516,18 +516,18 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="579679552"/>
+        <c:crossAx val="460766592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="579679552"/>
+        <c:axId val="460766592"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="10000000"/>
+          <c:max val="550000"/>
           <c:min val="30"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -577,7 +577,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="579685784"/>
+        <c:crossAx val="460767376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -591,6 +591,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -622,14 +623,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1227,7 +1228,7 @@
         <xdr:cNvPr id="4" name="Diagramm 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB80D08A-8F16-47F7-9AA2-FEFEC48B9453}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB80D08A-8F16-47F7-9AA2-FEFEC48B9453}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1249,18 +1250,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A05943FC-B791-489F-92F3-E0266273AAEB}" name="Tabelle3" displayName="Tabelle3" ref="B3:D16">
-  <autoFilter ref="B3:D16" xr:uid="{DCE1B6E3-F7C9-49C0-AA10-FAD00EDEF27F}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="B3:D16">
+  <autoFilter ref="B3:D16">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00AE56BD-0757-4AB5-8F21-D1BDAFD37FEF}" name="Datum" totalsRowLabel="Ergebnis" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{002C9410-77D0-43DB-9056-6E5A5C158D18}" name="Summe" dataDxfId="2">
+    <tableColumn id="1" name="Datum" totalsRowLabel="Ergebnis" dataDxfId="3"/>
+    <tableColumn id="2" name="Summe" dataDxfId="2">
       <calculatedColumnFormula>C3*2^(1.5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{06A8114D-F317-465F-97CA-101D5848C548}" name="Summe inkl. Mehrwertsteuer" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
+    <tableColumn id="3" name="Summe inkl. Mehrwertsteuer" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>ROUND(C4*(1+$B$2),2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1564,26 +1565,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570C504D-C406-4820-9805-346F1E16C9C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.41796875" customWidth="1"/>
-    <col min="5" max="5" width="11.20703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>0.19</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1594,7 +1595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>43831</v>
       </c>
@@ -1602,178 +1603,178 @@
         <v>30.99</v>
       </c>
       <c r="D4" s="3">
-        <f>ROUND(C4*(1+$B$2),2)</f>
+        <f t="shared" ref="D4:D16" si="0">ROUND(C4*(1+$B$2),2)</f>
         <v>36.880000000000003</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>43862</v>
       </c>
       <c r="C5" s="3">
-        <f>C4*2^(1.5)</f>
-        <v>87.652956595884419</v>
+        <f>C4*2^(1.15)</f>
+        <v>68.771115878765016</v>
       </c>
       <c r="D5" s="3">
-        <f>ROUND(C5*(1+$B$2),2)</f>
-        <v>104.31</v>
+        <f t="shared" si="0"/>
+        <v>81.84</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>43891</v>
       </c>
       <c r="C6" s="3">
-        <f>C5*2^(1.5)</f>
-        <v>247.91999999999993</v>
+        <f t="shared" ref="C6:C16" si="1">C5*2^(1.15)</f>
+        <v>152.61266147823576</v>
       </c>
       <c r="D6" s="3">
-        <f>ROUND(C6*(1+$B$2),2)</f>
-        <v>295.02</v>
+        <f t="shared" si="0"/>
+        <v>181.61</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>43922</v>
       </c>
       <c r="C7" s="3">
-        <f>C6*2^(1.5)</f>
-        <v>701.22365276707524</v>
+        <f t="shared" si="1"/>
+        <v>338.66870045454954</v>
       </c>
       <c r="D7" s="3">
-        <f>ROUND(C7*(1+$B$2),2)</f>
-        <v>834.46</v>
+        <f t="shared" si="0"/>
+        <v>403.02</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>43952</v>
       </c>
       <c r="C8" s="3">
-        <f>C7*2^(1.5)</f>
-        <v>1983.3599999999992</v>
+        <f t="shared" si="1"/>
+        <v>751.5529023385152</v>
       </c>
       <c r="D8" s="3">
-        <f>ROUND(C8*(1+$B$2),2)</f>
-        <v>2360.1999999999998</v>
+        <f t="shared" si="0"/>
+        <v>894.35</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>43983</v>
       </c>
       <c r="C9" s="3">
-        <f>C8*2^(1.5)</f>
-        <v>5609.789222136601</v>
+        <f t="shared" si="1"/>
+        <v>1667.8003141576057</v>
       </c>
       <c r="D9" s="3">
-        <f>ROUND(C9*(1+$B$2),2)</f>
-        <v>6675.65</v>
+        <f t="shared" si="0"/>
+        <v>1984.68</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>44013</v>
       </c>
       <c r="C10" s="3">
-        <f>C9*2^(1.5)</f>
-        <v>15866.879999999992</v>
+        <f t="shared" si="1"/>
+        <v>3701.0806281888808</v>
       </c>
       <c r="D10" s="3">
-        <f>ROUND(C10*(1+$B$2),2)</f>
-        <v>18881.59</v>
+        <f t="shared" si="0"/>
+        <v>4404.29</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>44044</v>
       </c>
       <c r="C11" s="3">
-        <f>C10*2^(1.5)</f>
-        <v>44878.313777092801</v>
+        <f t="shared" si="1"/>
+        <v>8213.2121574001285</v>
       </c>
       <c r="D11" s="3">
-        <f>ROUND(C11*(1+$B$2),2)</f>
-        <v>53405.19</v>
+        <f t="shared" si="0"/>
+        <v>9773.7199999999993</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>44075</v>
       </c>
       <c r="C12" s="3">
-        <f>C11*2^(1.5)</f>
-        <v>126935.03999999991</v>
+        <f t="shared" si="1"/>
+        <v>18226.258954935332</v>
       </c>
       <c r="D12" s="3">
-        <f>ROUND(C12*(1+$B$2),2)</f>
-        <v>151052.70000000001</v>
+        <f t="shared" si="0"/>
+        <v>21689.25</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>44105</v>
       </c>
       <c r="C13" s="3">
-        <f>C12*2^(1.5)</f>
-        <v>359026.51021674235</v>
+        <f t="shared" si="1"/>
+        <v>40446.601052798855</v>
       </c>
       <c r="D13" s="3">
-        <f>ROUND(C13*(1+$B$2),2)</f>
-        <v>427241.55</v>
+        <f t="shared" si="0"/>
+        <v>48131.46</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>44136</v>
       </c>
       <c r="C14" s="3">
-        <f>C13*2^(1.5)</f>
-        <v>1015480.3199999991</v>
+        <f t="shared" si="1"/>
+        <v>89756.627554185528</v>
       </c>
       <c r="D14" s="3">
-        <f>ROUND(C14*(1+$B$2),2)</f>
-        <v>1208421.58</v>
+        <f t="shared" si="0"/>
+        <v>106810.39</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>44166</v>
       </c>
       <c r="C15" s="3">
-        <f>C14*2^(1.5)</f>
-        <v>2872212.0817339383</v>
+        <f t="shared" si="1"/>
+        <v>199182.42769977564</v>
       </c>
       <c r="D15" s="3">
-        <f>ROUND(C15*(1+$B$2),2)</f>
-        <v>3417932.38</v>
+        <f t="shared" si="0"/>
+        <v>237027.09</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>44197</v>
       </c>
       <c r="C16" s="3">
-        <f>C15*2^(1.5)</f>
-        <v>8123842.5599999912</v>
+        <f t="shared" si="1"/>
+        <v>442013.48229606345</v>
       </c>
       <c r="D16" s="3">
-        <f>ROUND(C16*(1+$B$2),2)</f>
-        <v>9667372.6500000004</v>
+        <f t="shared" si="0"/>
+        <v>525996.04</v>
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>

</xml_diff>